<commit_message>
Highlighting on cells where order quantity is not zero
</commit_message>
<xml_diff>
--- a/Daily_Order_Report_2025-10-21.xlsx
+++ b/Daily_Order_Report_2025-10-21.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="176">
   <si>
     <t>Seg</t>
   </si>
@@ -502,28 +502,43 @@
     <t>Corporate Territory</t>
   </si>
   <si>
-    <t>Biman Bangladesh Airlines Limited</t>
-  </si>
-  <si>
-    <t>Manager (Commercial Store), Biman, H S I A Int'l Airport, Dhaka.</t>
+    <t>Confidence Electric Limited (Factory)</t>
+  </si>
+  <si>
+    <t>Mojompur, Taltola, Modonpur, Narayangonj</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Gazipur Territory</t>
+  </si>
+  <si>
+    <t>M/S Al - Mokka Enterprise (C)</t>
+  </si>
+  <si>
+    <t>Monipur, Gazipur Sador, Gazipur</t>
+  </si>
+  <si>
+    <t>01765140095, 01648936899</t>
+  </si>
+  <si>
+    <t>Container Territory</t>
+  </si>
+  <si>
+    <t>M/S Bright Renewables Ltd.</t>
+  </si>
+  <si>
+    <t>Sreepur, Mawna, Gazipur</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>OEM Territory</t>
-  </si>
-  <si>
-    <t>M/S MJS Corporation</t>
-  </si>
-  <si>
-    <t>Hobigonj Territory</t>
-  </si>
-  <si>
-    <t>M/S Al - Rafi Traders</t>
-  </si>
-  <si>
-    <t>Shoshan Road, Anowarpur, Habigonj</t>
+    <t>Confidence Group</t>
+  </si>
+  <si>
+    <t>Unique Trade Centre (UTC), Level 7, 08, Panthapath, Kawran Bazar, Dhaka 1215, Bangladesh</t>
   </si>
 </sst>
 </file>
@@ -1024,7 +1039,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DQ15"/>
+  <dimension ref="A1:DQ16"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="10" customWidth="1"/>
@@ -1165,8 +1180,12 @@
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="5">
+        <v>2</v>
+      </c>
+      <c r="C2" s="6">
+        <v>28500</v>
+      </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -1288,8 +1307,12 @@
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0</v>
+      </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -1411,8 +1434,12 @@
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
+      <c r="B4" s="5">
+        <v>2</v>
+      </c>
+      <c r="C4" s="6">
+        <v>22674</v>
+      </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -1534,8 +1561,12 @@
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
+      <c r="B5" s="5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6">
+        <v>46100</v>
+      </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -1657,8 +1688,12 @@
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="6"/>
+      <c r="B6" s="5">
+        <v>6</v>
+      </c>
+      <c r="C6" s="6">
+        <v>44102</v>
+      </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -1780,8 +1815,12 @@
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
+      <c r="B7" s="5">
+        <v>0</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0</v>
+      </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -1903,8 +1942,12 @@
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="6"/>
+      <c r="B8" s="5">
+        <v>0</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0</v>
+      </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -2027,10 +2070,10 @@
         <v>10</v>
       </c>
       <c r="B9" s="8">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C9" s="9">
-        <v>0</v>
+        <v>141376</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -3031,7 +3074,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="15">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="M13" s="15">
         <v>0</v>
@@ -3130,7 +3173,7 @@
         <v>0</v>
       </c>
       <c r="AS13" s="15">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AT13" s="15">
         <v>0</v>
@@ -3157,7 +3200,7 @@
         <v>0</v>
       </c>
       <c r="BB13" s="15">
-        <v>94</v>
+        <v>0</v>
       </c>
       <c r="BC13" s="15">
         <v>0</v>
@@ -3214,7 +3257,7 @@
         <v>0</v>
       </c>
       <c r="BU13" s="15">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="BV13" s="15">
         <v>0</v>
@@ -3372,10 +3415,10 @@
         <v>167</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F14" s="15">
         <v>0</v>
@@ -3384,7 +3427,7 @@
         <v>0</v>
       </c>
       <c r="H14" s="15">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I14" s="15">
         <v>0</v>
@@ -3405,7 +3448,7 @@
         <v>0</v>
       </c>
       <c r="O14" s="15">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="P14" s="15">
         <v>0</v>
@@ -3447,7 +3490,7 @@
         <v>0</v>
       </c>
       <c r="AC14" s="15">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="AD14" s="15">
         <v>0</v>
@@ -3480,7 +3523,7 @@
         <v>0</v>
       </c>
       <c r="AN14" s="15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO14" s="15">
         <v>0</v>
@@ -3522,7 +3565,7 @@
         <v>0</v>
       </c>
       <c r="BB14" s="15">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="BC14" s="15">
         <v>0</v>
@@ -3731,16 +3774,16 @@
         <v>3</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="F15" s="15">
         <v>0</v>
@@ -3749,7 +3792,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="15">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I15" s="15">
         <v>0</v>
@@ -3767,7 +3810,7 @@
         <v>0</v>
       </c>
       <c r="N15" s="15">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="O15" s="15">
         <v>0</v>
@@ -3908,149 +3951,149 @@
         <v>0</v>
       </c>
       <c r="BI15" s="15">
+        <v>0</v>
+      </c>
+      <c r="BJ15" s="15">
+        <v>0</v>
+      </c>
+      <c r="BK15" s="15">
+        <v>0</v>
+      </c>
+      <c r="BL15" s="15">
+        <v>0</v>
+      </c>
+      <c r="BM15" s="15">
+        <v>0</v>
+      </c>
+      <c r="BN15" s="15">
+        <v>0</v>
+      </c>
+      <c r="BO15" s="15">
+        <v>0</v>
+      </c>
+      <c r="BP15" s="15">
+        <v>0</v>
+      </c>
+      <c r="BQ15" s="15">
+        <v>0</v>
+      </c>
+      <c r="BR15" s="15">
+        <v>0</v>
+      </c>
+      <c r="BS15" s="15">
+        <v>0</v>
+      </c>
+      <c r="BT15" s="15">
+        <v>0</v>
+      </c>
+      <c r="BU15" s="15">
+        <v>0</v>
+      </c>
+      <c r="BV15" s="15">
+        <v>0</v>
+      </c>
+      <c r="BW15" s="15">
+        <v>0</v>
+      </c>
+      <c r="BX15" s="15">
+        <v>0</v>
+      </c>
+      <c r="BY15" s="15">
+        <v>0</v>
+      </c>
+      <c r="BZ15" s="15">
+        <v>0</v>
+      </c>
+      <c r="CA15" s="15">
+        <v>0</v>
+      </c>
+      <c r="CB15" s="15">
+        <v>0</v>
+      </c>
+      <c r="CC15" s="15">
+        <v>0</v>
+      </c>
+      <c r="CD15" s="15">
+        <v>0</v>
+      </c>
+      <c r="CE15" s="15">
+        <v>0</v>
+      </c>
+      <c r="CF15" s="15">
+        <v>0</v>
+      </c>
+      <c r="CG15" s="15">
+        <v>0</v>
+      </c>
+      <c r="CH15" s="15">
+        <v>0</v>
+      </c>
+      <c r="CI15" s="15">
+        <v>0</v>
+      </c>
+      <c r="CJ15" s="15">
+        <v>0</v>
+      </c>
+      <c r="CK15" s="15">
+        <v>0</v>
+      </c>
+      <c r="CL15" s="15">
+        <v>0</v>
+      </c>
+      <c r="CM15" s="15">
+        <v>0</v>
+      </c>
+      <c r="CN15" s="15">
+        <v>0</v>
+      </c>
+      <c r="CO15" s="15">
+        <v>0</v>
+      </c>
+      <c r="CP15" s="15">
+        <v>0</v>
+      </c>
+      <c r="CQ15" s="15">
+        <v>0</v>
+      </c>
+      <c r="CR15" s="15">
+        <v>0</v>
+      </c>
+      <c r="CS15" s="15">
+        <v>0</v>
+      </c>
+      <c r="CT15" s="15">
+        <v>0</v>
+      </c>
+      <c r="CU15" s="15">
+        <v>0</v>
+      </c>
+      <c r="CV15" s="15">
+        <v>0</v>
+      </c>
+      <c r="CW15" s="15">
+        <v>0</v>
+      </c>
+      <c r="CX15" s="15">
+        <v>0</v>
+      </c>
+      <c r="CY15" s="15">
+        <v>0</v>
+      </c>
+      <c r="CZ15" s="15">
+        <v>0</v>
+      </c>
+      <c r="DA15" s="15">
+        <v>0</v>
+      </c>
+      <c r="DB15" s="15">
+        <v>0</v>
+      </c>
+      <c r="DC15" s="15">
+        <v>0</v>
+      </c>
+      <c r="DD15" s="15">
         <v>2</v>
       </c>
-      <c r="BJ15" s="15">
-        <v>0</v>
-      </c>
-      <c r="BK15" s="15">
-        <v>0</v>
-      </c>
-      <c r="BL15" s="15">
-        <v>0</v>
-      </c>
-      <c r="BM15" s="15">
-        <v>0</v>
-      </c>
-      <c r="BN15" s="15">
-        <v>0</v>
-      </c>
-      <c r="BO15" s="15">
-        <v>0</v>
-      </c>
-      <c r="BP15" s="15">
-        <v>0</v>
-      </c>
-      <c r="BQ15" s="15">
-        <v>0</v>
-      </c>
-      <c r="BR15" s="15">
-        <v>0</v>
-      </c>
-      <c r="BS15" s="15">
-        <v>0</v>
-      </c>
-      <c r="BT15" s="15">
-        <v>0</v>
-      </c>
-      <c r="BU15" s="15">
-        <v>0</v>
-      </c>
-      <c r="BV15" s="15">
-        <v>0</v>
-      </c>
-      <c r="BW15" s="15">
-        <v>0</v>
-      </c>
-      <c r="BX15" s="15">
-        <v>0</v>
-      </c>
-      <c r="BY15" s="15">
-        <v>0</v>
-      </c>
-      <c r="BZ15" s="15">
-        <v>0</v>
-      </c>
-      <c r="CA15" s="15">
-        <v>0</v>
-      </c>
-      <c r="CB15" s="15">
-        <v>0</v>
-      </c>
-      <c r="CC15" s="15">
-        <v>0</v>
-      </c>
-      <c r="CD15" s="15">
-        <v>0</v>
-      </c>
-      <c r="CE15" s="15">
-        <v>0</v>
-      </c>
-      <c r="CF15" s="15">
-        <v>0</v>
-      </c>
-      <c r="CG15" s="15">
-        <v>0</v>
-      </c>
-      <c r="CH15" s="15">
-        <v>0</v>
-      </c>
-      <c r="CI15" s="15">
-        <v>0</v>
-      </c>
-      <c r="CJ15" s="15">
-        <v>0</v>
-      </c>
-      <c r="CK15" s="15">
-        <v>0</v>
-      </c>
-      <c r="CL15" s="15">
-        <v>0</v>
-      </c>
-      <c r="CM15" s="15">
-        <v>0</v>
-      </c>
-      <c r="CN15" s="15">
-        <v>0</v>
-      </c>
-      <c r="CO15" s="15">
-        <v>0</v>
-      </c>
-      <c r="CP15" s="15">
-        <v>0</v>
-      </c>
-      <c r="CQ15" s="15">
-        <v>0</v>
-      </c>
-      <c r="CR15" s="15">
-        <v>0</v>
-      </c>
-      <c r="CS15" s="15">
-        <v>0</v>
-      </c>
-      <c r="CT15" s="15">
-        <v>0</v>
-      </c>
-      <c r="CU15" s="15">
-        <v>0</v>
-      </c>
-      <c r="CV15" s="15">
-        <v>0</v>
-      </c>
-      <c r="CW15" s="15">
-        <v>0</v>
-      </c>
-      <c r="CX15" s="15">
-        <v>0</v>
-      </c>
-      <c r="CY15" s="15">
-        <v>0</v>
-      </c>
-      <c r="CZ15" s="15">
-        <v>0</v>
-      </c>
-      <c r="DA15" s="15">
-        <v>0</v>
-      </c>
-      <c r="DB15" s="15">
-        <v>0</v>
-      </c>
-      <c r="DC15" s="15">
-        <v>0</v>
-      </c>
-      <c r="DD15" s="15">
-        <v>0</v>
-      </c>
       <c r="DE15" s="15">
         <v>0</v>
       </c>
@@ -4058,10 +4101,10 @@
         <v>0</v>
       </c>
       <c r="DG15" s="15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="DH15" s="15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="DI15" s="15">
         <v>0</v>
@@ -4088,6 +4131,371 @@
         <v>0</v>
       </c>
       <c r="DQ15" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:121" x14ac:dyDescent="0.25">
+      <c r="A16" s="14">
+        <v>4</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="F16" s="15">
+        <v>0</v>
+      </c>
+      <c r="G16" s="15">
+        <v>0</v>
+      </c>
+      <c r="H16" s="15">
+        <v>0</v>
+      </c>
+      <c r="I16" s="15">
+        <v>0</v>
+      </c>
+      <c r="J16" s="15">
+        <v>0</v>
+      </c>
+      <c r="K16" s="15">
+        <v>0</v>
+      </c>
+      <c r="L16" s="15">
+        <v>0</v>
+      </c>
+      <c r="M16" s="15">
+        <v>0</v>
+      </c>
+      <c r="N16" s="15">
+        <v>0</v>
+      </c>
+      <c r="O16" s="15">
+        <v>0</v>
+      </c>
+      <c r="P16" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="15">
+        <v>0</v>
+      </c>
+      <c r="R16" s="15">
+        <v>0</v>
+      </c>
+      <c r="S16" s="15">
+        <v>0</v>
+      </c>
+      <c r="T16" s="15">
+        <v>0</v>
+      </c>
+      <c r="U16" s="15">
+        <v>0</v>
+      </c>
+      <c r="V16" s="15">
+        <v>0</v>
+      </c>
+      <c r="W16" s="15">
+        <v>0</v>
+      </c>
+      <c r="X16" s="15">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="15">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AE16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AF16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AG16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AK16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AL16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AM16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AN16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AO16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AP16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AQ16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AR16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AS16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AT16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AU16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AV16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AW16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AX16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AY16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AZ16" s="15">
+        <v>0</v>
+      </c>
+      <c r="BA16" s="15">
+        <v>0</v>
+      </c>
+      <c r="BB16" s="15">
+        <v>0</v>
+      </c>
+      <c r="BC16" s="15">
+        <v>0</v>
+      </c>
+      <c r="BD16" s="15">
+        <v>0</v>
+      </c>
+      <c r="BE16" s="15">
+        <v>0</v>
+      </c>
+      <c r="BF16" s="15">
+        <v>0</v>
+      </c>
+      <c r="BG16" s="15">
+        <v>0</v>
+      </c>
+      <c r="BH16" s="15">
+        <v>0</v>
+      </c>
+      <c r="BI16" s="15">
+        <v>0</v>
+      </c>
+      <c r="BJ16" s="15">
+        <v>0</v>
+      </c>
+      <c r="BK16" s="15">
+        <v>0</v>
+      </c>
+      <c r="BL16" s="15">
+        <v>0</v>
+      </c>
+      <c r="BM16" s="15">
+        <v>0</v>
+      </c>
+      <c r="BN16" s="15">
+        <v>0</v>
+      </c>
+      <c r="BO16" s="15">
+        <v>0</v>
+      </c>
+      <c r="BP16" s="15">
+        <v>0</v>
+      </c>
+      <c r="BQ16" s="15">
+        <v>0</v>
+      </c>
+      <c r="BR16" s="15">
+        <v>0</v>
+      </c>
+      <c r="BS16" s="15">
+        <v>0</v>
+      </c>
+      <c r="BT16" s="15">
+        <v>0</v>
+      </c>
+      <c r="BU16" s="15">
+        <v>0</v>
+      </c>
+      <c r="BV16" s="15">
+        <v>0</v>
+      </c>
+      <c r="BW16" s="15">
+        <v>0</v>
+      </c>
+      <c r="BX16" s="15">
+        <v>0</v>
+      </c>
+      <c r="BY16" s="15">
+        <v>0</v>
+      </c>
+      <c r="BZ16" s="15">
+        <v>0</v>
+      </c>
+      <c r="CA16" s="15">
+        <v>0</v>
+      </c>
+      <c r="CB16" s="15">
+        <v>0</v>
+      </c>
+      <c r="CC16" s="15">
+        <v>0</v>
+      </c>
+      <c r="CD16" s="15">
+        <v>0</v>
+      </c>
+      <c r="CE16" s="15">
+        <v>0</v>
+      </c>
+      <c r="CF16" s="15">
+        <v>0</v>
+      </c>
+      <c r="CG16" s="15">
+        <v>0</v>
+      </c>
+      <c r="CH16" s="15">
+        <v>0</v>
+      </c>
+      <c r="CI16" s="15">
+        <v>2</v>
+      </c>
+      <c r="CJ16" s="15">
+        <v>0</v>
+      </c>
+      <c r="CK16" s="15">
+        <v>0</v>
+      </c>
+      <c r="CL16" s="15">
+        <v>0</v>
+      </c>
+      <c r="CM16" s="15">
+        <v>0</v>
+      </c>
+      <c r="CN16" s="15">
+        <v>0</v>
+      </c>
+      <c r="CO16" s="15">
+        <v>2</v>
+      </c>
+      <c r="CP16" s="15">
+        <v>0</v>
+      </c>
+      <c r="CQ16" s="15">
+        <v>0</v>
+      </c>
+      <c r="CR16" s="15">
+        <v>0</v>
+      </c>
+      <c r="CS16" s="15">
+        <v>0</v>
+      </c>
+      <c r="CT16" s="15">
+        <v>0</v>
+      </c>
+      <c r="CU16" s="15">
+        <v>0</v>
+      </c>
+      <c r="CV16" s="15">
+        <v>0</v>
+      </c>
+      <c r="CW16" s="15">
+        <v>0</v>
+      </c>
+      <c r="CX16" s="15">
+        <v>0</v>
+      </c>
+      <c r="CY16" s="15">
+        <v>0</v>
+      </c>
+      <c r="CZ16" s="15">
+        <v>0</v>
+      </c>
+      <c r="DA16" s="15">
+        <v>0</v>
+      </c>
+      <c r="DB16" s="15">
+        <v>0</v>
+      </c>
+      <c r="DC16" s="15">
+        <v>0</v>
+      </c>
+      <c r="DD16" s="15">
+        <v>0</v>
+      </c>
+      <c r="DE16" s="15">
+        <v>0</v>
+      </c>
+      <c r="DF16" s="15">
+        <v>0</v>
+      </c>
+      <c r="DG16" s="15">
+        <v>0</v>
+      </c>
+      <c r="DH16" s="15">
+        <v>0</v>
+      </c>
+      <c r="DI16" s="15">
+        <v>0</v>
+      </c>
+      <c r="DJ16" s="15">
+        <v>0</v>
+      </c>
+      <c r="DK16" s="15">
+        <v>0</v>
+      </c>
+      <c r="DL16" s="15">
+        <v>0</v>
+      </c>
+      <c r="DM16" s="15">
+        <v>0</v>
+      </c>
+      <c r="DN16" s="15">
+        <v>0</v>
+      </c>
+      <c r="DO16" s="15">
+        <v>0</v>
+      </c>
+      <c r="DP16" s="15">
+        <v>0</v>
+      </c>
+      <c r="DQ16" s="15">
         <v>0</v>
       </c>
     </row>

</xml_diff>